<commit_message>
Added Entry for participant data folder and validation
Signed-off-by: Julian-Webb <julian.webb00@gmail.com>
</commit_message>
<xml_diff>
--- a/data/test_participant/stimulation_order.xlsx
+++ b/data/test_participant/stimulation_order.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\PycharmProjects\EvokingSensation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\PycharmProjects\EvokingSensation\data\test_participant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E4DA7-08CC-4FB5-8055-CADEEA067EE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4B5156-8F16-4265-8A73-4CDA359459F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,24 +34,6 @@
     <t>electrodes</t>
   </si>
   <si>
-    <t>[1, 8, 6, 5, 4, 7, 3]</t>
-  </si>
-  <si>
-    <t>[5, 7, 2, 6, 4, 1]</t>
-  </si>
-  <si>
-    <t>[2, 7, 4]</t>
-  </si>
-  <si>
-    <t>[(1, 2), (15, 16), (11, 12), (9, 10), (7, 8), (13, 14), (5, 6)]</t>
-  </si>
-  <si>
-    <t>[(9, 10), (13, 14), (3, 4), (11, 12), (7, 8), (1, 2)]</t>
-  </si>
-  <si>
-    <t>[(3, 4), (13, 14), (7, 8)]</t>
-  </si>
-  <si>
     <t>overall trial</t>
   </si>
   <si>
@@ -59,6 +41,24 @@
   </si>
   <si>
     <t>[(1, 2), (3, 4)]</t>
+  </si>
+  <si>
+    <t>[(1, 2)]</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>[(3, 4)]</t>
+  </si>
+  <si>
+    <t>[2, 1]</t>
+  </si>
+  <si>
+    <t>[(3, 4), (1, 2)]</t>
   </si>
 </sst>
 </file>
@@ -82,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,12 +92,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE5FFE5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5E5FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -129,13 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +470,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +482,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -515,10 +508,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -529,47 +522,47 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A trial is now repeated if a stimulator error occurs
Signed-off-by: Julian-Webb <julian.webb00@gmail.com>
</commit_message>
<xml_diff>
--- a/data/test_participant/stimulation_order.xlsx
+++ b/data/test_participant/stimulation_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\PycharmProjects\EvokingSensation\data\test_participant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4B5156-8F16-4265-8A73-4CDA359459F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F85B311-C65C-4535-A920-F1A995721D6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>block</t>
   </si>
@@ -40,25 +40,16 @@
     <t>[1, 2]</t>
   </si>
   <si>
-    <t>[(1, 2), (3, 4)]</t>
-  </si>
-  <si>
-    <t>[(1, 2)]</t>
-  </si>
-  <si>
     <t>[1]</t>
   </si>
   <si>
-    <t>[2]</t>
-  </si>
-  <si>
-    <t>[(3, 4)]</t>
-  </si>
-  <si>
-    <t>[2, 1]</t>
-  </si>
-  <si>
-    <t>[(3, 4), (1, 2)]</t>
+    <t>[(0,0)]</t>
+  </si>
+  <si>
+    <t>[1, 2, 3]</t>
+  </si>
+  <si>
+    <t>[3]</t>
   </si>
 </sst>
 </file>
@@ -470,7 +461,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -525,10 +516,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -542,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>7</v>
@@ -559,10 +550,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a timer to the End of block screen and continuing is only possible after it runs out
Signed-off-by: Julian-Webb <julian.webb00@gmail.com>
</commit_message>
<xml_diff>
--- a/data/test_participant/stimulation_order.xlsx
+++ b/data/test_participant/stimulation_order.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\PycharmProjects\EvokingSensation\data\test_participant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\PycharmProjects\EvokingSensation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F85B311-C65C-4535-A920-F1A995721D6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E4DA7-08CC-4FB5-8055-CADEEA067EE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>block</t>
   </si>
@@ -34,22 +34,31 @@
     <t>electrodes</t>
   </si>
   <si>
+    <t>[1, 8, 6, 5, 4, 7, 3]</t>
+  </si>
+  <si>
+    <t>[5, 7, 2, 6, 4, 1]</t>
+  </si>
+  <si>
+    <t>[2, 7, 4]</t>
+  </si>
+  <si>
+    <t>[(1, 2), (15, 16), (11, 12), (9, 10), (7, 8), (13, 14), (5, 6)]</t>
+  </si>
+  <si>
+    <t>[(9, 10), (13, 14), (3, 4), (11, 12), (7, 8), (1, 2)]</t>
+  </si>
+  <si>
+    <t>[(3, 4), (13, 14), (7, 8)]</t>
+  </si>
+  <si>
     <t>overall trial</t>
   </si>
   <si>
     <t>[1, 2]</t>
   </si>
   <si>
-    <t>[1]</t>
-  </si>
-  <si>
-    <t>[(0,0)]</t>
-  </si>
-  <si>
-    <t>[1, 2, 3]</t>
-  </si>
-  <si>
-    <t>[3]</t>
+    <t>[(1, 2), (3, 4)]</t>
   </si>
 </sst>
 </file>
@@ -73,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +92,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE5FFE5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5E5FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -114,12 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +477,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,7 +489,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -499,10 +515,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -513,10 +529,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
@@ -526,34 +542,34 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added options for different channel-electrode-maps
Signed-off-by: Julian-Webb <julian.webb00@gmail.com>
</commit_message>
<xml_diff>
--- a/data/test_participant/stimulation_order.xlsx
+++ b/data/test_participant/stimulation_order.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\PycharmProjects\EvokingSensation\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E4DA7-08CC-4FB5-8055-CADEEA067EE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="StimulationOrder" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>block</t>
   </si>
@@ -31,41 +25,50 @@
     <t>channels</t>
   </si>
   <si>
+    <t>channel_electrode_map_id</t>
+  </si>
+  <si>
     <t>electrodes</t>
   </si>
   <si>
-    <t>[1, 8, 6, 5, 4, 7, 3]</t>
-  </si>
-  <si>
-    <t>[5, 7, 2, 6, 4, 1]</t>
-  </si>
-  <si>
-    <t>[2, 7, 4]</t>
-  </si>
-  <si>
-    <t>[(1, 2), (15, 16), (11, 12), (9, 10), (7, 8), (13, 14), (5, 6)]</t>
-  </si>
-  <si>
-    <t>[(9, 10), (13, 14), (3, 4), (11, 12), (7, 8), (1, 2)]</t>
-  </si>
-  <si>
-    <t>[(3, 4), (13, 14), (7, 8)]</t>
-  </si>
-  <si>
     <t>overall trial</t>
   </si>
   <si>
-    <t>[1, 2]</t>
-  </si>
-  <si>
-    <t>[(1, 2), (3, 4)]</t>
+    <t>[8, 1]</t>
+  </si>
+  <si>
+    <t>[8]</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>vertical</t>
+  </si>
+  <si>
+    <t>[(15, 16), (1, 2)]</t>
+  </si>
+  <si>
+    <t>[(15, 16)]</t>
+  </si>
+  <si>
+    <t>[(1, 2)]</t>
+  </si>
+  <si>
+    <t>[(12, 16), (1, 5)]</t>
+  </si>
+  <si>
+    <t>[(1, 5)]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,13 +94,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE5FFE5"/>
+        <fgColor rgb="FFE5E5FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE5E5FF"/>
+        <fgColor rgb="FFE5FFE5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,14 +145,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -196,7 +191,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,27 +223,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,24 +257,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -473,23 +432,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
-    <col min="5" max="5" width="71.88671875" customWidth="1"/>
+    <col min="2" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -503,8 +461,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -515,61 +476,153 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>